<commit_message>
Updated Mack/MW to multi-period
Updated Tyche code to calculate the multi-period Mack and Merz-Wuethrich error terms.
Also added some more example triangles.
</commit_message>
<xml_diff>
--- a/Analytic/Triangles.xlsx
+++ b/Analytic/Triangles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="990" windowWidth="22605" windowHeight="12840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="TaylorAshe" sheetId="1" r:id="rId1"/>
-    <sheet name="Example1" sheetId="2" r:id="rId2"/>
-    <sheet name="Example2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sanders" sheetId="8" r:id="rId2"/>
+    <sheet name="MerzWuethrich" sheetId="9" r:id="rId3"/>
+    <sheet name="Example1" sheetId="2" r:id="rId4"/>
+    <sheet name="Example2" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Example1">Example1!$B$2:$L$12</definedName>
     <definedName name="Example1_Indicator">Example1!$B$15:$K$24</definedName>
     <definedName name="Example2">Example2!$B$2:$L$12</definedName>
     <definedName name="Example2_Indicator">Example2!$B$15:$K$24</definedName>
+    <definedName name="MerzWuethrich">MerzWuethrich!$B$2:$S$19</definedName>
+    <definedName name="MerzWuethrich_Indicator">MerzWuethrich!$B$22:$R$38</definedName>
+    <definedName name="Sanders">Sanders!$B$2:$K$11</definedName>
+    <definedName name="Sanders_Indicator">Sanders!$B$14:$J$22</definedName>
     <definedName name="TaylorAshe">TaylorAshe!$B$2:$L$12</definedName>
     <definedName name="TaylorAshe_Indicator">TaylorAshe!$B$15:$K$24</definedName>
     <definedName name="TestShape1">#REF!</definedName>
@@ -32,7 +38,7 @@
     <definedName name="TestShape4">#REF!</definedName>
     <definedName name="TestShape4_Indicator">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,12 +53,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>https://people.math.ethz.ch/~wueth/Papers/data.csv</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +97,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -863,13 +888,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L24"/>
+  <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1</v>
       </c>
@@ -897,257 +922,245 @@
       <c r="K2">
         <v>9</v>
       </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2007</v>
       </c>
       <c r="C3">
-        <v>5946975.4500000002</v>
+        <v>58046</v>
       </c>
       <c r="D3">
-        <v>9668212.0350000001</v>
+        <v>127970</v>
       </c>
       <c r="E3">
-        <v>10563929.324999999</v>
+        <v>476599</v>
       </c>
       <c r="F3">
-        <v>10771689.654999999</v>
+        <v>1027692</v>
       </c>
       <c r="G3">
-        <v>10978393.645</v>
+        <v>1360489</v>
       </c>
       <c r="H3">
-        <v>11040517.795</v>
+        <v>1647310</v>
       </c>
       <c r="I3">
-        <v>11106331.215</v>
+        <v>1819179</v>
       </c>
       <c r="J3">
-        <v>11121180.875</v>
+        <v>1906852</v>
       </c>
       <c r="K3">
-        <v>11132310.404999999</v>
-      </c>
-      <c r="L3">
-        <v>11148123.824999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+        <v>1950105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2008</v>
       </c>
       <c r="C4">
-        <v>6346756.1210883399</v>
+        <v>24492</v>
       </c>
       <c r="D4">
-        <v>9593161.7102224305</v>
+        <v>141767</v>
       </c>
       <c r="E4">
-        <v>10316383.4555893</v>
+        <v>984288</v>
       </c>
       <c r="F4">
-        <v>10468180.234918799</v>
+        <v>2142656</v>
       </c>
       <c r="G4">
-        <v>10536004.3278106</v>
+        <v>2961978</v>
       </c>
       <c r="H4">
-        <v>10572607.8065142</v>
+        <v>3683940</v>
       </c>
       <c r="I4">
-        <v>10625359.8787634</v>
+        <v>4048898</v>
       </c>
       <c r="J4">
-        <v>10636546.271505499</v>
-      </c>
-      <c r="K4">
-        <v>10648191.8006816</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+        <v>4115760</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2009</v>
       </c>
       <c r="C5">
-        <v>6269090.2112323297</v>
+        <v>32848</v>
       </c>
       <c r="D5">
-        <v>9245313.2727096993</v>
+        <v>274682</v>
       </c>
       <c r="E5">
-        <v>10092365.9687528</v>
+        <v>1522637</v>
       </c>
       <c r="F5">
-        <v>10355134.2883568</v>
+        <v>3203427</v>
       </c>
       <c r="G5">
-        <v>10507837.3872965</v>
+        <v>4445927</v>
       </c>
       <c r="H5">
-        <v>10573281.572556401</v>
+        <v>5158781</v>
       </c>
       <c r="I5">
-        <v>10626826.815041799</v>
-      </c>
-      <c r="J5">
-        <v>10635751.0221227</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+        <v>5342585</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2010</v>
       </c>
       <c r="C6">
-        <v>5863014.8075402202</v>
+        <v>21439</v>
       </c>
       <c r="D6">
-        <v>8546239.1100235395</v>
+        <v>529828</v>
       </c>
       <c r="E6">
-        <v>9268770.8317457791</v>
+        <v>2900301</v>
       </c>
       <c r="F6">
-        <v>9459423.5571675301</v>
+        <v>4999019</v>
       </c>
       <c r="G6">
-        <v>9592399.1507406104</v>
+        <v>6460112</v>
       </c>
       <c r="H6">
-        <v>9680739.5800374094</v>
-      </c>
-      <c r="I6">
-        <v>9724068.2097572591</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+        <v>6853904</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2011</v>
       </c>
       <c r="C7">
-        <v>5778885.3596461304</v>
+        <v>40397</v>
       </c>
       <c r="D7">
-        <v>8524114.2689106409</v>
+        <v>763394</v>
       </c>
       <c r="E7">
-        <v>9178008.6292282697</v>
+        <v>2920745</v>
       </c>
       <c r="F7">
-        <v>9451404.1160852108</v>
+        <v>4989572</v>
       </c>
       <c r="G7">
-        <v>9681691.6721275505</v>
-      </c>
-      <c r="H7">
-        <v>9786916.0519487802</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+        <v>5648563</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2012</v>
       </c>
       <c r="C8">
-        <v>6184793.3995723603</v>
+        <v>90748</v>
       </c>
       <c r="D8">
-        <v>9013131.8745357301</v>
+        <v>951994</v>
       </c>
       <c r="E8">
-        <v>9585896.6549400408</v>
+        <v>4210640</v>
       </c>
       <c r="F8">
-        <v>9830796.08111641</v>
-      </c>
-      <c r="G8">
-        <v>9935752.9780491404</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+        <v>5866482</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2013</v>
       </c>
       <c r="C9">
-        <v>5600184.3963173702</v>
+        <v>62096</v>
       </c>
       <c r="D9">
-        <v>8493391.2994029503</v>
+        <v>868480</v>
       </c>
       <c r="E9">
-        <v>9056505.2100427896</v>
-      </c>
-      <c r="F9">
-        <v>9282022.2196497805</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+        <v>1954797</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2014</v>
       </c>
       <c r="C10">
-        <v>5288065.6150194705</v>
+        <v>24983</v>
       </c>
       <c r="D10">
-        <v>7728168.7972333897</v>
-      </c>
-      <c r="E10">
-        <v>8256211.3572572796</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+        <v>284441</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2015</v>
       </c>
       <c r="C11">
-        <v>5290792.9454416102</v>
-      </c>
-      <c r="D11">
-        <v>7648728.9110740302</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>2016</v>
-      </c>
-      <c r="C12">
-        <v>5675568.1390453298</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>13121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2007</v>
+      </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>8</v>
-      </c>
-      <c r="K15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1170,16 +1183,10 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1199,16 +1206,10 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1225,16 +1226,10 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1248,16 +1243,10 @@
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1268,16 +1257,10 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1285,43 +1268,12 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>2014</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>2015</v>
-      </c>
-      <c r="C24">
         <v>1</v>
       </c>
     </row>
@@ -1331,6 +1283,1162 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <v>13</v>
+      </c>
+      <c r="P2">
+        <v>14</v>
+      </c>
+      <c r="Q2">
+        <v>15</v>
+      </c>
+      <c r="R2">
+        <v>16</v>
+      </c>
+      <c r="S2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2003</v>
+      </c>
+      <c r="C3">
+        <v>13109</v>
+      </c>
+      <c r="D3">
+        <v>20355</v>
+      </c>
+      <c r="E3">
+        <v>21337</v>
+      </c>
+      <c r="F3">
+        <v>22043</v>
+      </c>
+      <c r="G3">
+        <v>22401</v>
+      </c>
+      <c r="H3">
+        <v>22658</v>
+      </c>
+      <c r="I3">
+        <v>22997</v>
+      </c>
+      <c r="J3">
+        <v>23158</v>
+      </c>
+      <c r="K3">
+        <v>23492</v>
+      </c>
+      <c r="L3">
+        <v>23664</v>
+      </c>
+      <c r="M3">
+        <v>23699</v>
+      </c>
+      <c r="N3">
+        <v>23904</v>
+      </c>
+      <c r="O3">
+        <v>23960</v>
+      </c>
+      <c r="P3">
+        <v>23992</v>
+      </c>
+      <c r="Q3">
+        <v>23994</v>
+      </c>
+      <c r="R3">
+        <v>24001</v>
+      </c>
+      <c r="S3">
+        <v>24002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2004</v>
+      </c>
+      <c r="C4">
+        <v>14457</v>
+      </c>
+      <c r="D4">
+        <v>22038</v>
+      </c>
+      <c r="E4">
+        <v>22627</v>
+      </c>
+      <c r="F4">
+        <v>23114</v>
+      </c>
+      <c r="G4">
+        <v>23238</v>
+      </c>
+      <c r="H4">
+        <v>23312</v>
+      </c>
+      <c r="I4">
+        <v>23440</v>
+      </c>
+      <c r="J4">
+        <v>23490</v>
+      </c>
+      <c r="K4">
+        <v>23964</v>
+      </c>
+      <c r="L4">
+        <v>23976</v>
+      </c>
+      <c r="M4">
+        <v>24048</v>
+      </c>
+      <c r="N4">
+        <v>24111</v>
+      </c>
+      <c r="O4">
+        <v>24252</v>
+      </c>
+      <c r="P4">
+        <v>24538</v>
+      </c>
+      <c r="Q4">
+        <v>24540</v>
+      </c>
+      <c r="R4">
+        <v>24550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2005</v>
+      </c>
+      <c r="C5">
+        <v>16075</v>
+      </c>
+      <c r="D5">
+        <v>22672</v>
+      </c>
+      <c r="E5">
+        <v>23753</v>
+      </c>
+      <c r="F5">
+        <v>24052</v>
+      </c>
+      <c r="G5">
+        <v>24206</v>
+      </c>
+      <c r="H5">
+        <v>24757</v>
+      </c>
+      <c r="I5">
+        <v>24786</v>
+      </c>
+      <c r="J5">
+        <v>24807</v>
+      </c>
+      <c r="K5">
+        <v>24823</v>
+      </c>
+      <c r="L5">
+        <v>24888</v>
+      </c>
+      <c r="M5">
+        <v>24986</v>
+      </c>
+      <c r="N5">
+        <v>25401</v>
+      </c>
+      <c r="O5">
+        <v>25681</v>
+      </c>
+      <c r="P5">
+        <v>25705</v>
+      </c>
+      <c r="Q5">
+        <v>25732</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2006</v>
+      </c>
+      <c r="C6">
+        <v>15682</v>
+      </c>
+      <c r="D6">
+        <v>23464</v>
+      </c>
+      <c r="E6">
+        <v>24465</v>
+      </c>
+      <c r="F6">
+        <v>25052</v>
+      </c>
+      <c r="G6">
+        <v>25529</v>
+      </c>
+      <c r="H6">
+        <v>25708</v>
+      </c>
+      <c r="I6">
+        <v>25752</v>
+      </c>
+      <c r="J6">
+        <v>25770</v>
+      </c>
+      <c r="K6">
+        <v>25835</v>
+      </c>
+      <c r="L6">
+        <v>26075</v>
+      </c>
+      <c r="M6">
+        <v>26082</v>
+      </c>
+      <c r="N6">
+        <v>26146</v>
+      </c>
+      <c r="O6">
+        <v>26150</v>
+      </c>
+      <c r="P6">
+        <v>26167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2007</v>
+      </c>
+      <c r="C7">
+        <v>16551</v>
+      </c>
+      <c r="D7">
+        <v>23706</v>
+      </c>
+      <c r="E7">
+        <v>24627</v>
+      </c>
+      <c r="F7">
+        <v>25573</v>
+      </c>
+      <c r="G7">
+        <v>26046</v>
+      </c>
+      <c r="H7">
+        <v>26115</v>
+      </c>
+      <c r="I7">
+        <v>26283</v>
+      </c>
+      <c r="J7">
+        <v>26481</v>
+      </c>
+      <c r="K7">
+        <v>26701</v>
+      </c>
+      <c r="L7">
+        <v>26718</v>
+      </c>
+      <c r="M7">
+        <v>26724</v>
+      </c>
+      <c r="N7">
+        <v>26728</v>
+      </c>
+      <c r="O7">
+        <v>26735</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2008</v>
+      </c>
+      <c r="C8">
+        <v>15439</v>
+      </c>
+      <c r="D8">
+        <v>23796</v>
+      </c>
+      <c r="E8">
+        <v>24866</v>
+      </c>
+      <c r="F8">
+        <v>25317</v>
+      </c>
+      <c r="G8">
+        <v>26139</v>
+      </c>
+      <c r="H8">
+        <v>26154</v>
+      </c>
+      <c r="I8">
+        <v>26175</v>
+      </c>
+      <c r="J8">
+        <v>26205</v>
+      </c>
+      <c r="K8">
+        <v>26764</v>
+      </c>
+      <c r="L8">
+        <v>26818</v>
+      </c>
+      <c r="M8">
+        <v>26836</v>
+      </c>
+      <c r="N8">
+        <v>26959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2009</v>
+      </c>
+      <c r="C9">
+        <v>14629</v>
+      </c>
+      <c r="D9">
+        <v>21645</v>
+      </c>
+      <c r="E9">
+        <v>22826</v>
+      </c>
+      <c r="F9">
+        <v>23599</v>
+      </c>
+      <c r="G9">
+        <v>24992</v>
+      </c>
+      <c r="H9">
+        <v>25434</v>
+      </c>
+      <c r="I9">
+        <v>25476</v>
+      </c>
+      <c r="J9">
+        <v>25549</v>
+      </c>
+      <c r="K9">
+        <v>25604</v>
+      </c>
+      <c r="L9">
+        <v>25709</v>
+      </c>
+      <c r="M9">
+        <v>25723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2010</v>
+      </c>
+      <c r="C10">
+        <v>17585</v>
+      </c>
+      <c r="D10">
+        <v>26288</v>
+      </c>
+      <c r="E10">
+        <v>27623</v>
+      </c>
+      <c r="F10">
+        <v>27939</v>
+      </c>
+      <c r="G10">
+        <v>28335</v>
+      </c>
+      <c r="H10">
+        <v>28638</v>
+      </c>
+      <c r="I10">
+        <v>28715</v>
+      </c>
+      <c r="J10">
+        <v>28759</v>
+      </c>
+      <c r="K10">
+        <v>29525</v>
+      </c>
+      <c r="L10">
+        <v>30302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2011</v>
+      </c>
+      <c r="C11">
+        <v>17419</v>
+      </c>
+      <c r="D11">
+        <v>25941</v>
+      </c>
+      <c r="E11">
+        <v>27066</v>
+      </c>
+      <c r="F11">
+        <v>27761</v>
+      </c>
+      <c r="G11">
+        <v>28043</v>
+      </c>
+      <c r="H11">
+        <v>28477</v>
+      </c>
+      <c r="I11">
+        <v>28721</v>
+      </c>
+      <c r="J11">
+        <v>28878</v>
+      </c>
+      <c r="K11">
+        <v>28948</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2012</v>
+      </c>
+      <c r="C12">
+        <v>16665</v>
+      </c>
+      <c r="D12">
+        <v>25370</v>
+      </c>
+      <c r="E12">
+        <v>26909</v>
+      </c>
+      <c r="F12">
+        <v>27611</v>
+      </c>
+      <c r="G12">
+        <v>27729</v>
+      </c>
+      <c r="H12">
+        <v>27861</v>
+      </c>
+      <c r="I12">
+        <v>29830</v>
+      </c>
+      <c r="J12">
+        <v>29844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2013</v>
+      </c>
+      <c r="C13">
+        <v>15471</v>
+      </c>
+      <c r="D13">
+        <v>23745</v>
+      </c>
+      <c r="E13">
+        <v>25117</v>
+      </c>
+      <c r="F13">
+        <v>26378</v>
+      </c>
+      <c r="G13">
+        <v>26971</v>
+      </c>
+      <c r="H13">
+        <v>27396</v>
+      </c>
+      <c r="I13">
+        <v>27480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2014</v>
+      </c>
+      <c r="C14">
+        <v>15103</v>
+      </c>
+      <c r="D14">
+        <v>23393</v>
+      </c>
+      <c r="E14">
+        <v>26809</v>
+      </c>
+      <c r="F14">
+        <v>27691</v>
+      </c>
+      <c r="G14">
+        <v>28061</v>
+      </c>
+      <c r="H14">
+        <v>29183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2015</v>
+      </c>
+      <c r="C15">
+        <v>14540</v>
+      </c>
+      <c r="D15">
+        <v>22642</v>
+      </c>
+      <c r="E15">
+        <v>23571</v>
+      </c>
+      <c r="F15">
+        <v>24127</v>
+      </c>
+      <c r="G15">
+        <v>24210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2016</v>
+      </c>
+      <c r="C16">
+        <v>14590</v>
+      </c>
+      <c r="D16">
+        <v>22336</v>
+      </c>
+      <c r="E16">
+        <v>23440</v>
+      </c>
+      <c r="F16">
+        <v>24029</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2017</v>
+      </c>
+      <c r="C17">
+        <v>13967</v>
+      </c>
+      <c r="D17">
+        <v>21515</v>
+      </c>
+      <c r="E17">
+        <v>22603</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2018</v>
+      </c>
+      <c r="C18">
+        <v>12930</v>
+      </c>
+      <c r="D18">
+        <v>20111</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2019</v>
+      </c>
+      <c r="C19">
+        <v>12539</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>13</v>
+      </c>
+      <c r="P22">
+        <v>14</v>
+      </c>
+      <c r="Q22">
+        <v>15</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2003</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2004</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2005</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2006</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2007</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2008</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2009</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2010</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>2011</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>2012</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2013</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>2014</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2015</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>2016</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>2017</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>2018</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L24"/>
   <sheetViews>
@@ -1375,6 +2483,475 @@
         <v>2007</v>
       </c>
       <c r="C3">
+        <v>5946975.4500000002</v>
+      </c>
+      <c r="D3">
+        <v>9668212.0350000001</v>
+      </c>
+      <c r="E3">
+        <v>10563929.324999999</v>
+      </c>
+      <c r="F3">
+        <v>10771689.654999999</v>
+      </c>
+      <c r="G3">
+        <v>10978393.645</v>
+      </c>
+      <c r="H3">
+        <v>11040517.795</v>
+      </c>
+      <c r="I3">
+        <v>11106331.215</v>
+      </c>
+      <c r="J3">
+        <v>11121180.875</v>
+      </c>
+      <c r="K3">
+        <v>11132310.404999999</v>
+      </c>
+      <c r="L3">
+        <v>11148123.824999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2008</v>
+      </c>
+      <c r="C4">
+        <v>6346756.1210883399</v>
+      </c>
+      <c r="D4">
+        <v>9593161.7102224305</v>
+      </c>
+      <c r="E4">
+        <v>10316383.4555893</v>
+      </c>
+      <c r="F4">
+        <v>10468180.234918799</v>
+      </c>
+      <c r="G4">
+        <v>10536004.3278106</v>
+      </c>
+      <c r="H4">
+        <v>10572607.8065142</v>
+      </c>
+      <c r="I4">
+        <v>10625359.8787634</v>
+      </c>
+      <c r="J4">
+        <v>10636546.271505499</v>
+      </c>
+      <c r="K4">
+        <v>10648191.8006816</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2009</v>
+      </c>
+      <c r="C5">
+        <v>6269090.2112323297</v>
+      </c>
+      <c r="D5">
+        <v>9245313.2727096993</v>
+      </c>
+      <c r="E5">
+        <v>10092365.9687528</v>
+      </c>
+      <c r="F5">
+        <v>10355134.2883568</v>
+      </c>
+      <c r="G5">
+        <v>10507837.3872965</v>
+      </c>
+      <c r="H5">
+        <v>10573281.572556401</v>
+      </c>
+      <c r="I5">
+        <v>10626826.815041799</v>
+      </c>
+      <c r="J5">
+        <v>10635751.0221227</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2010</v>
+      </c>
+      <c r="C6">
+        <v>5863014.8075402202</v>
+      </c>
+      <c r="D6">
+        <v>8546239.1100235395</v>
+      </c>
+      <c r="E6">
+        <v>9268770.8317457791</v>
+      </c>
+      <c r="F6">
+        <v>9459423.5571675301</v>
+      </c>
+      <c r="G6">
+        <v>9592399.1507406104</v>
+      </c>
+      <c r="H6">
+        <v>9680739.5800374094</v>
+      </c>
+      <c r="I6">
+        <v>9724068.2097572591</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2011</v>
+      </c>
+      <c r="C7">
+        <v>5778885.3596461304</v>
+      </c>
+      <c r="D7">
+        <v>8524114.2689106409</v>
+      </c>
+      <c r="E7">
+        <v>9178008.6292282697</v>
+      </c>
+      <c r="F7">
+        <v>9451404.1160852108</v>
+      </c>
+      <c r="G7">
+        <v>9681691.6721275505</v>
+      </c>
+      <c r="H7">
+        <v>9786916.0519487802</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2012</v>
+      </c>
+      <c r="C8">
+        <v>6184793.3995723603</v>
+      </c>
+      <c r="D8">
+        <v>9013131.8745357301</v>
+      </c>
+      <c r="E8">
+        <v>9585896.6549400408</v>
+      </c>
+      <c r="F8">
+        <v>9830796.08111641</v>
+      </c>
+      <c r="G8">
+        <v>9935752.9780491404</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2013</v>
+      </c>
+      <c r="C9">
+        <v>5600184.3963173702</v>
+      </c>
+      <c r="D9">
+        <v>8493391.2994029503</v>
+      </c>
+      <c r="E9">
+        <v>9056505.2100427896</v>
+      </c>
+      <c r="F9">
+        <v>9282022.2196497805</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2014</v>
+      </c>
+      <c r="C10">
+        <v>5288065.6150194705</v>
+      </c>
+      <c r="D10">
+        <v>7728168.7972333897</v>
+      </c>
+      <c r="E10">
+        <v>8256211.3572572796</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2015</v>
+      </c>
+      <c r="C11">
+        <v>5290792.9454416102</v>
+      </c>
+      <c r="D11">
+        <v>7648728.9110740302</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2016</v>
+      </c>
+      <c r="C12">
+        <v>5675568.1390453298</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2007</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2008</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2009</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2010</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2011</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2012</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2013</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2014</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2015</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2007</v>
+      </c>
+      <c r="C3">
         <v>184</v>
       </c>
       <c r="D3">

</xml_diff>